<commit_message>
update image specs generator
</commit_message>
<xml_diff>
--- a/0_dev/99_image-specs-generator.xlsx
+++ b/0_dev/99_image-specs-generator.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/undiscipliningvc/0_dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D688D6FF-BC2D-6440-A0BD-032FE119F26B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E3C1EE-8330-BC49-B87A-31CBEEAF99E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="24940" windowHeight="15000" activeTab="1" xr2:uid="{0FB4BD1C-FF0F-3F40-B68C-098FE484C6E0}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="24940" windowHeight="15000" activeTab="3" xr2:uid="{0FB4BD1C-FF0F-3F40-B68C-098FE484C6E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Carousel" sheetId="3" r:id="rId1"/>
     <sheet name="Home Reg" sheetId="2" r:id="rId2"/>
-    <sheet name="Zoomcast" sheetId="1" r:id="rId3"/>
+    <sheet name="Zoomcast" sheetId="4" r:id="rId3"/>
+    <sheet name="Biographies" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="4">
-  <si>
-    <t>img/zoomcasts/xxx-</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="5">
   <si>
     <t>px.jpg</t>
   </si>
@@ -47,7 +45,13 @@
     <t xml:space="preserve">w, </t>
   </si>
   <si>
-    <t>img/home/000X-deriv-</t>
+    <t>/img/about/xxx-</t>
+  </si>
+  <si>
+    <t>/img/zoomcasts/xxx-</t>
+  </si>
+  <si>
+    <t>/img/home/000X-deriv-</t>
   </si>
 </sst>
 </file>
@@ -402,7 +406,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B1" sqref="B1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -412,17 +416,17 @@
         <v>1800</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" t="str">
         <f t="shared" ref="E1:E11" si="0">B1&amp;A1&amp;C1&amp;" "&amp;A1&amp;D1</f>
-        <v xml:space="preserve">img/home/000X-deriv-1800px.jpg 1800w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-1800px.jpg 1800w, </v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -430,17 +434,17 @@
         <v>1650</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-1650px.jpg 1650w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-1650px.jpg 1650w, </v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -448,17 +452,17 @@
         <v>1500</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-1500px.jpg 1500w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-1500px.jpg 1500w, </v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -466,17 +470,17 @@
         <v>1350</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-1350px.jpg 1350w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-1350px.jpg 1350w, </v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -484,17 +488,17 @@
         <v>1200</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-1200px.jpg 1200w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-1200px.jpg 1200w, </v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -502,17 +506,17 @@
         <v>1050</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-1050px.jpg 1050w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-1050px.jpg 1050w, </v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -520,17 +524,17 @@
         <v>900</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-900px.jpg 900w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-900px.jpg 900w, </v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -538,17 +542,17 @@
         <v>750</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-750px.jpg 750w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-750px.jpg 750w, </v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -556,17 +560,17 @@
         <v>600</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-600px.jpg 600w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-600px.jpg 600w, </v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -574,17 +578,17 @@
         <v>450</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-450px.jpg 450w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-450px.jpg 450w, </v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -592,23 +596,23 @@
         <v>300</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-300px.jpg 300w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-300px.jpg 300w, </v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>E1&amp;E2&amp;E3&amp;E4&amp;E5&amp;E6&amp;E7&amp;E8&amp;E9&amp;E10&amp;E11</f>
-        <v xml:space="preserve">img/home/000X-deriv-1800px.jpg 1800w, img/home/000X-deriv-1650px.jpg 1650w, img/home/000X-deriv-1500px.jpg 1500w, img/home/000X-deriv-1350px.jpg 1350w, img/home/000X-deriv-1200px.jpg 1200w, img/home/000X-deriv-1050px.jpg 1050w, img/home/000X-deriv-900px.jpg 900w, img/home/000X-deriv-750px.jpg 750w, img/home/000X-deriv-600px.jpg 600w, img/home/000X-deriv-450px.jpg 450w, img/home/000X-deriv-300px.jpg 300w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-1800px.jpg 1800w, /img/home/000X-deriv-1650px.jpg 1650w, /img/home/000X-deriv-1500px.jpg 1500w, /img/home/000X-deriv-1350px.jpg 1350w, /img/home/000X-deriv-1200px.jpg 1200w, /img/home/000X-deriv-1050px.jpg 1050w, /img/home/000X-deriv-900px.jpg 900w, /img/home/000X-deriv-750px.jpg 750w, /img/home/000X-deriv-600px.jpg 600w, /img/home/000X-deriv-450px.jpg 450w, /img/home/000X-deriv-300px.jpg 300w, </v>
       </c>
     </row>
   </sheetData>
@@ -620,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34CFEC6-58FB-3648-8FB2-DBFB0F2FED03}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,17 +635,17 @@
         <v>1170</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" t="str">
         <f t="shared" ref="E1:E6" si="0">B1&amp;A1&amp;C1&amp;" "&amp;A1&amp;D1</f>
-        <v xml:space="preserve">img/home/000X-deriv-1170px.jpg 1170w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-1170px.jpg 1170w, </v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -649,17 +653,17 @@
         <v>888</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-888px.jpg 888w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-888px.jpg 888w, </v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -667,17 +671,17 @@
         <v>585</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-585px.jpg 585w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-585px.jpg 585w, </v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -685,17 +689,17 @@
         <v>568</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-568px.jpg 568w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-568px.jpg 568w, </v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -703,17 +707,17 @@
         <v>444</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-444px.jpg 444w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-444px.jpg 444w, </v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -721,23 +725,23 @@
         <v>284</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/home/000X-deriv-284px.jpg 284w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-284px.jpg 284w, </v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>E1&amp;E2&amp;E3&amp;E4&amp;E5&amp;E6</f>
-        <v xml:space="preserve">img/home/000X-deriv-1170px.jpg 1170w, img/home/000X-deriv-888px.jpg 888w, img/home/000X-deriv-585px.jpg 585w, img/home/000X-deriv-568px.jpg 568w, img/home/000X-deriv-444px.jpg 444w, img/home/000X-deriv-284px.jpg 284w, </v>
+        <v xml:space="preserve">/img/home/000X-deriv-1170px.jpg 1170w, /img/home/000X-deriv-888px.jpg 888w, /img/home/000X-deriv-585px.jpg 585w, /img/home/000X-deriv-568px.jpg 568w, /img/home/000X-deriv-444px.jpg 444w, /img/home/000X-deriv-284px.jpg 284w, </v>
       </c>
     </row>
   </sheetData>
@@ -749,11 +753,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5042EA8F-7AE2-8141-ABB3-C8DC23691D78}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A228DC4-093A-4F4F-B8F8-388E163AF1CF}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,17 +767,17 @@
         <v>1275</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" t="str">
         <f>B1&amp;A1&amp;C1&amp;" "&amp;A1&amp;D1</f>
-        <v xml:space="preserve">img/zoomcasts/xxx-1275px.jpg 1275w, </v>
+        <v xml:space="preserve">/img/zoomcasts/xxx-1275px.jpg 1275w, </v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -781,17 +785,17 @@
         <v>930</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" ref="E2:E8" si="0">B2&amp;A2&amp;C2&amp;" "&amp;A2&amp;D2</f>
-        <v xml:space="preserve">img/zoomcasts/xxx-930px.jpg 930w, </v>
+        <v xml:space="preserve">/img/zoomcasts/xxx-930px.jpg 930w, </v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -799,17 +803,17 @@
         <v>816</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/zoomcasts/xxx-816px.jpg 816w, </v>
+        <v xml:space="preserve">/img/zoomcasts/xxx-816px.jpg 816w, </v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -817,17 +821,17 @@
         <v>663</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/zoomcasts/xxx-663px.jpg 663w, </v>
+        <v xml:space="preserve">/img/zoomcasts/xxx-663px.jpg 663w, </v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -835,17 +839,17 @@
         <v>532</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/zoomcasts/xxx-532px.jpg 532w, </v>
+        <v xml:space="preserve">/img/zoomcasts/xxx-532px.jpg 532w, </v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -853,17 +857,17 @@
         <v>465</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/zoomcasts/xxx-465px.jpg 465w, </v>
+        <v xml:space="preserve">/img/zoomcasts/xxx-465px.jpg 465w, </v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -871,17 +875,17 @@
         <v>408</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/zoomcasts/xxx-408px.jpg 408w, </v>
+        <v xml:space="preserve">/img/zoomcasts/xxx-408px.jpg 408w, </v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -889,23 +893,188 @@
         <v>266</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">img/zoomcasts/xxx-266px.jpg 266w, </v>
+        <v xml:space="preserve">/img/zoomcasts/xxx-266px.jpg 266w, </v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>E1&amp;E2&amp;E3&amp;E4&amp;E5&amp;E6&amp;E7&amp;E8</f>
-        <v xml:space="preserve">img/zoomcasts/xxx-1275px.jpg 1275w, img/zoomcasts/xxx-930px.jpg 930w, img/zoomcasts/xxx-816px.jpg 816w, img/zoomcasts/xxx-663px.jpg 663w, img/zoomcasts/xxx-532px.jpg 532w, img/zoomcasts/xxx-465px.jpg 465w, img/zoomcasts/xxx-408px.jpg 408w, img/zoomcasts/xxx-266px.jpg 266w, </v>
+        <v xml:space="preserve">/img/zoomcasts/xxx-1275px.jpg 1275w, /img/zoomcasts/xxx-930px.jpg 930w, /img/zoomcasts/xxx-816px.jpg 816w, /img/zoomcasts/xxx-663px.jpg 663w, /img/zoomcasts/xxx-532px.jpg 532w, /img/zoomcasts/xxx-465px.jpg 465w, /img/zoomcasts/xxx-408px.jpg 408w, /img/zoomcasts/xxx-266px.jpg 266w, </v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5042EA8F-7AE2-8141-ABB3-C8DC23691D78}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>570</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="str">
+        <f>B1&amp;A1&amp;C1&amp;" "&amp;A1&amp;D1</f>
+        <v xml:space="preserve">/img/about/xxx-570px.jpg 570w, </v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>446</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E8" si="0">B2&amp;A2&amp;C2&amp;" "&amp;A2&amp;D2</f>
+        <v xml:space="preserve">/img/about/xxx-446px.jpg 446w, </v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>390</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/img/about/xxx-390px.jpg 390w, </v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>350</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/img/about/xxx-350px.jpg 350w, </v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>285</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/img/about/xxx-285px.jpg 285w, </v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>223</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/img/about/xxx-223px.jpg 223w, </v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>195</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/img/about/xxx-195px.jpg 195w, </v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/img/about/xxx-175px.jpg 175w, </v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>E1&amp;E2&amp;E3&amp;E4&amp;E5&amp;E6&amp;E7&amp;E8</f>
+        <v xml:space="preserve">/img/about/xxx-570px.jpg 570w, /img/about/xxx-446px.jpg 446w, /img/about/xxx-390px.jpg 390w, /img/about/xxx-350px.jpg 350w, /img/about/xxx-285px.jpg 285w, /img/about/xxx-223px.jpg 223w, /img/about/xxx-195px.jpg 195w, /img/about/xxx-175px.jpg 175w, </v>
       </c>
     </row>
   </sheetData>

</xml_diff>